<commit_message>
Increase Health and Shield cost
</commit_message>
<xml_diff>
--- a/Design Note - Cost balancing.xlsx
+++ b/Design Note - Cost balancing.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="58">
   <si>
     <t>Locomotion</t>
   </si>
@@ -116,33 +116,9 @@
     <t>Level</t>
   </si>
   <si>
-    <t>Min</t>
-  </si>
-  <si>
     <t>MinTotal</t>
   </si>
   <si>
-    <t>Max</t>
-  </si>
-  <si>
-    <t>MaxTotal</t>
-  </si>
-  <si>
-    <t>Min spend: You use revolvers for as long as possible or get an early machine pistol and stick with it. You don't heal.</t>
-  </si>
-  <si>
-    <t>Rich</t>
-  </si>
-  <si>
-    <t>RichTotal</t>
-  </si>
-  <si>
-    <t>Rich spend: You buy a mag for one new gun at each level, eventually settling on one machine pistol and one back-up. You heal twice.</t>
-  </si>
-  <si>
-    <t>Max spend: You fully kit-out two machine pistols and heal twice. Should only be possible in Endless mode.</t>
-  </si>
-  <si>
     <t>Median</t>
   </si>
   <si>
@@ -161,19 +137,73 @@
     <t>(End)</t>
   </si>
   <si>
-    <t>Interesting spend: An interesting play-through where you've had to prioritise your purchases, missing out on some non-essentials. You can heal once, but if you don't, those points can buy a lot of things.</t>
-  </si>
-  <si>
-    <t>Interesting</t>
-  </si>
-  <si>
-    <t>InterestingTotal</t>
-  </si>
-  <si>
     <t>Shield</t>
   </si>
   <si>
     <t>Bayonet</t>
+  </si>
+  <si>
+    <t>Minimalist</t>
+  </si>
+  <si>
+    <t>MachinePistol</t>
+  </si>
+  <si>
+    <t>Spending as little as possible. You get a muzzle brake and a laser to improve your shooting, and your capacity improves as the guns improve.</t>
+  </si>
+  <si>
+    <t>Machine pistol</t>
+  </si>
+  <si>
+    <t>You save up in the early game so that you can get a great machine pistol at the end.</t>
+  </si>
+  <si>
+    <t>Minimalist Healing</t>
+  </si>
+  <si>
+    <t>Machine pistol Healing</t>
+  </si>
+  <si>
+    <t>Above, but healing once.</t>
+  </si>
+  <si>
+    <t>MaPi Healing</t>
+  </si>
+  <si>
+    <t>Min Healing</t>
+  </si>
+  <si>
+    <t>MinHe Total</t>
+  </si>
+  <si>
+    <t>MaPi Total</t>
+  </si>
+  <si>
+    <t>MaPiHe Total</t>
+  </si>
+  <si>
+    <t>Token value</t>
+  </si>
+  <si>
+    <t>Base price (3)</t>
+  </si>
+  <si>
+    <t>Health price (6)</t>
+  </si>
+  <si>
+    <t>Ideal</t>
+  </si>
+  <si>
+    <t>Base price (1)</t>
+  </si>
+  <si>
+    <t>Shield price (4)</t>
+  </si>
+  <si>
+    <t>Health price (3)</t>
+  </si>
+  <si>
+    <t>Shield price (9)</t>
   </si>
 </sst>
 </file>
@@ -294,7 +324,58 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="10">
+    <dxf>
+      <font>
+        <color theme="2"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2"/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -596,7 +677,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -604,10 +685,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:M24"/>
+  <dimension ref="B2:N24"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView topLeftCell="B1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -615,15 +696,16 @@
     <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="4.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="9.140625" style="11"/>
+    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="12.5703125" customWidth="1"/>
+    <col min="10" max="10" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>20</v>
       </c>
@@ -634,32 +716,37 @@
         <v>22</v>
       </c>
       <c r="E2" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="I2" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="J2" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="F2" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="G2" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="H2" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="I2" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="J2" s="11" t="s">
-        <v>45</v>
-      </c>
       <c r="K2" s="11" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="L2" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="M2" s="11"/>
-    </row>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+      <c r="M2" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="N2" s="11" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -673,32 +760,39 @@
         <v>0</v>
       </c>
       <c r="F3" s="11">
-        <v>1</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3">
-        <v>2</v>
-      </c>
-      <c r="I3" s="12">
+        <v>0</v>
+      </c>
+      <c r="G3" s="11">
+        <v>0</v>
+      </c>
+      <c r="H3" s="11">
+        <v>0</v>
+      </c>
+      <c r="I3" s="11">
+        <v>0</v>
+      </c>
+      <c r="J3" s="12">
         <f>D3*E3</f>
         <v>0</v>
       </c>
-      <c r="J3" s="12">
+      <c r="K3" s="12">
         <f>F3*D3</f>
-        <v>1</v>
-      </c>
-      <c r="K3" s="11">
+        <v>0</v>
+      </c>
+      <c r="L3" s="12">
         <f>G3*D3</f>
         <v>0</v>
       </c>
-      <c r="L3" s="11">
+      <c r="M3" s="12">
         <f>H3*D3</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="N3" s="11">
+        <f>I3*D3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
@@ -712,32 +806,39 @@
         <v>0</v>
       </c>
       <c r="F4" s="11">
-        <v>1</v>
-      </c>
-      <c r="G4">
-        <v>2</v>
-      </c>
-      <c r="H4">
-        <v>2</v>
-      </c>
-      <c r="I4" s="12">
-        <f>D4*E4</f>
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="G4" s="11">
+        <v>0</v>
+      </c>
+      <c r="H4" s="11">
+        <v>0</v>
+      </c>
+      <c r="I4" s="11">
+        <v>1</v>
       </c>
       <c r="J4" s="12">
-        <f>F4*D4</f>
-        <v>1</v>
-      </c>
-      <c r="K4" s="11">
-        <f>G4*D4</f>
-        <v>2</v>
-      </c>
-      <c r="L4" s="11">
-        <f>H4*D4</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
+        <f t="shared" ref="J4:J15" si="0">D4*E4</f>
+        <v>0</v>
+      </c>
+      <c r="K4" s="12">
+        <f t="shared" ref="K4:K15" si="1">F4*D4</f>
+        <v>0</v>
+      </c>
+      <c r="L4" s="12">
+        <f t="shared" ref="L4:L15" si="2">G4*D4</f>
+        <v>0</v>
+      </c>
+      <c r="M4" s="12">
+        <f t="shared" ref="M4:M14" si="3">H4*D4</f>
+        <v>0</v>
+      </c>
+      <c r="N4" s="11">
+        <f t="shared" ref="N4:N15" si="4">I4*D4</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>3</v>
       </c>
@@ -753,30 +854,37 @@
       <c r="F5" s="11">
         <v>1</v>
       </c>
-      <c r="G5">
-        <v>1</v>
-      </c>
-      <c r="H5">
-        <v>1</v>
-      </c>
-      <c r="I5" s="12">
-        <f>D5*E5</f>
+      <c r="G5" s="11">
+        <v>1</v>
+      </c>
+      <c r="H5" s="11">
+        <v>1</v>
+      </c>
+      <c r="I5" s="11">
         <v>1</v>
       </c>
       <c r="J5" s="12">
-        <f>F5*D5</f>
-        <v>1</v>
-      </c>
-      <c r="K5" s="11">
-        <f>G5*D5</f>
-        <v>1</v>
-      </c>
-      <c r="L5" s="11">
-        <f>H5*D5</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K5" s="12">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="L5" s="12">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="M5" s="12">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="N5" s="11">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>3</v>
       </c>
@@ -792,35 +900,42 @@
       <c r="F6" s="11">
         <v>0</v>
       </c>
-      <c r="G6">
-        <v>1</v>
-      </c>
-      <c r="H6">
-        <v>1</v>
-      </c>
-      <c r="I6" s="12">
-        <f>D6*E6</f>
+      <c r="G6" s="11">
+        <v>0</v>
+      </c>
+      <c r="H6" s="11">
+        <v>0</v>
+      </c>
+      <c r="I6" s="11">
         <v>0</v>
       </c>
       <c r="J6" s="12">
-        <f>F6*D6</f>
-        <v>0</v>
-      </c>
-      <c r="K6" s="11">
-        <f>G6*D6</f>
-        <v>1</v>
-      </c>
-      <c r="L6" s="11">
-        <f>H6*D6</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K6" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L6" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M6" s="12">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="N6" s="11">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="D7" s="7">
         <v>1</v>
@@ -831,30 +946,37 @@
       <c r="F7" s="11">
         <v>0</v>
       </c>
-      <c r="G7">
-        <v>1</v>
-      </c>
-      <c r="H7">
-        <v>2</v>
-      </c>
-      <c r="I7" s="12">
-        <f>D7*E7</f>
+      <c r="G7" s="11">
+        <v>0</v>
+      </c>
+      <c r="H7" s="11">
+        <v>0</v>
+      </c>
+      <c r="I7" s="11">
         <v>0</v>
       </c>
       <c r="J7" s="12">
-        <f>F7*D7</f>
-        <v>0</v>
-      </c>
-      <c r="K7" s="11">
-        <f>G7*D7</f>
-        <v>1</v>
-      </c>
-      <c r="L7" s="11">
-        <f>H7*D7</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K7" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L7" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M7" s="12">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="N7" s="11">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
         <v>6</v>
       </c>
@@ -868,32 +990,39 @@
         <v>0</v>
       </c>
       <c r="F8" s="11">
-        <v>1</v>
-      </c>
-      <c r="G8">
-        <v>1</v>
-      </c>
-      <c r="H8">
-        <v>2</v>
-      </c>
-      <c r="I8" s="12">
-        <f>D8*E8</f>
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="G8" s="11">
+        <v>1</v>
+      </c>
+      <c r="H8" s="11">
+        <v>1</v>
+      </c>
+      <c r="I8" s="11">
+        <v>1</v>
       </c>
       <c r="J8" s="12">
-        <f>F8*D8</f>
-        <v>1</v>
-      </c>
-      <c r="K8" s="11">
-        <f>G8*D8</f>
-        <v>1</v>
-      </c>
-      <c r="L8" s="11">
-        <f>H8*D8</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K8" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L8" s="12">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="M8" s="12">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="N8" s="11">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
         <v>6</v>
       </c>
@@ -904,35 +1033,42 @@
         <v>1</v>
       </c>
       <c r="E9" s="11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F9" s="11">
-        <v>1</v>
-      </c>
-      <c r="G9">
-        <v>1</v>
-      </c>
-      <c r="H9">
-        <v>2</v>
-      </c>
-      <c r="I9" s="12">
-        <f>D9*E9</f>
+        <v>0</v>
+      </c>
+      <c r="G9" s="11">
+        <v>1</v>
+      </c>
+      <c r="H9" s="11">
+        <v>1</v>
+      </c>
+      <c r="I9" s="11">
         <v>1</v>
       </c>
       <c r="J9" s="12">
-        <f>F9*D9</f>
-        <v>1</v>
-      </c>
-      <c r="K9" s="11">
-        <f>G9*D9</f>
-        <v>1</v>
-      </c>
-      <c r="L9" s="11">
-        <f>H9*D9</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K9" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L9" s="12">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="M9" s="12">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="N9" s="11">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B10" s="4" t="s">
         <v>9</v>
       </c>
@@ -946,32 +1082,39 @@
         <v>1</v>
       </c>
       <c r="F10" s="11">
-        <v>0</v>
-      </c>
-      <c r="G10">
-        <v>2</v>
-      </c>
-      <c r="H10">
-        <v>2</v>
-      </c>
-      <c r="I10" s="12">
-        <f>D10*E10</f>
+        <v>1</v>
+      </c>
+      <c r="G10" s="11">
+        <v>0</v>
+      </c>
+      <c r="H10" s="11">
+        <v>0</v>
+      </c>
+      <c r="I10" s="11">
         <v>1</v>
       </c>
       <c r="J10" s="12">
-        <f>F10*D10</f>
-        <v>0</v>
-      </c>
-      <c r="K10" s="11">
-        <f>G10*D10</f>
-        <v>2</v>
-      </c>
-      <c r="L10" s="11">
-        <f>H10*D10</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K10" s="12">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="L10" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M10" s="12">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="N10" s="11">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B11" s="4" t="s">
         <v>9</v>
       </c>
@@ -987,30 +1130,37 @@
       <c r="F11" s="11">
         <v>0</v>
       </c>
-      <c r="G11">
-        <v>1</v>
-      </c>
-      <c r="H11">
-        <v>2</v>
-      </c>
-      <c r="I11" s="12">
-        <f>D11*E11</f>
+      <c r="G11" s="11">
+        <v>0</v>
+      </c>
+      <c r="H11" s="11">
+        <v>0</v>
+      </c>
+      <c r="I11" s="11">
         <v>0</v>
       </c>
       <c r="J11" s="12">
-        <f>F11*D11</f>
-        <v>0</v>
-      </c>
-      <c r="K11" s="11">
-        <f>G11*D11</f>
-        <v>1</v>
-      </c>
-      <c r="L11" s="11">
-        <f>H11*D11</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K11" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L11" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M11" s="12">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="N11" s="11">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
         <v>12</v>
       </c>
@@ -1018,7 +1168,7 @@
         <v>13</v>
       </c>
       <c r="D12" s="10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E12" s="11">
         <v>0</v>
@@ -1026,38 +1176,45 @@
       <c r="F12" s="11">
         <v>1</v>
       </c>
-      <c r="G12">
-        <v>2</v>
-      </c>
-      <c r="H12">
-        <v>2</v>
-      </c>
-      <c r="I12" s="12">
-        <f>D12*E12</f>
+      <c r="G12" s="11">
+        <v>0</v>
+      </c>
+      <c r="H12" s="11">
+        <v>1</v>
+      </c>
+      <c r="I12" s="11">
         <v>0</v>
       </c>
       <c r="J12" s="12">
-        <f>F12*D12</f>
-        <v>2</v>
-      </c>
-      <c r="K12" s="11">
-        <f>G12*D12</f>
-        <v>4</v>
-      </c>
-      <c r="L12" s="11">
-        <f>H12*D12</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K12" s="12">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="L12" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M12" s="12">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="N12" s="11">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="D13" s="10">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E13" s="11">
         <v>0</v>
@@ -1065,30 +1222,37 @@
       <c r="F13" s="11">
         <v>0</v>
       </c>
-      <c r="G13">
-        <v>1</v>
-      </c>
-      <c r="H13">
-        <v>1</v>
-      </c>
-      <c r="I13" s="12">
-        <f>D13*E13</f>
+      <c r="G13" s="11">
+        <v>0</v>
+      </c>
+      <c r="H13" s="11">
+        <v>0</v>
+      </c>
+      <c r="I13" s="11">
         <v>0</v>
       </c>
       <c r="J13" s="12">
-        <f>F13*D13</f>
-        <v>0</v>
-      </c>
-      <c r="K13" s="11">
-        <f>G13*D13</f>
-        <v>2</v>
-      </c>
-      <c r="L13" s="11">
-        <f>H13*D13</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K13" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L13" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M13" s="12">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="N13" s="11">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>23</v>
       </c>
@@ -1096,35 +1260,42 @@
         <v>2</v>
       </c>
       <c r="E14" s="11">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F14" s="11">
-        <v>3</v>
-      </c>
-      <c r="G14">
         <v>5</v>
       </c>
-      <c r="H14">
+      <c r="G14" s="11">
+        <v>4</v>
+      </c>
+      <c r="H14" s="11">
+        <v>4</v>
+      </c>
+      <c r="I14" s="11">
+        <v>4</v>
+      </c>
+      <c r="J14" s="12">
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="I14" s="11">
-        <f>D14*E14</f>
-        <v>6</v>
-      </c>
-      <c r="J14" s="12">
-        <f>F14*D14</f>
-        <v>6</v>
-      </c>
-      <c r="K14" s="11">
-        <f>G14*D14</f>
+      <c r="K14" s="12">
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="L14" s="11">
-        <f>H14*D14</f>
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="L14" s="12">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="M14" s="12">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="N14" s="11">
+        <f t="shared" si="4"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>24</v>
       </c>
@@ -1132,92 +1303,120 @@
         <v>3</v>
       </c>
       <c r="E15" s="11">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F15" s="11">
-        <v>4</v>
-      </c>
-      <c r="G15">
-        <v>4</v>
-      </c>
-      <c r="H15">
-        <v>8</v>
+        <v>0</v>
+      </c>
+      <c r="G15" s="11">
+        <v>3</v>
+      </c>
+      <c r="H15" s="11">
+        <v>3</v>
       </c>
       <c r="I15" s="11">
-        <f>D15*E15</f>
+        <v>3</v>
+      </c>
+      <c r="J15" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K15" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L15" s="12">
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
-      <c r="J15" s="12">
-        <f>F15*D15</f>
-        <v>12</v>
-      </c>
-      <c r="K15" s="11">
-        <f>G15*D15</f>
-        <v>12</v>
-      </c>
-      <c r="L15" s="11">
+      <c r="M15" s="12">
         <f>H15*D15</f>
-        <v>24</v>
-      </c>
-    </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="N15" s="11">
+        <f t="shared" si="4"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
       <c r="D17" t="s">
         <v>25</v>
       </c>
-      <c r="H17" s="11"/>
-      <c r="I17" s="11">
-        <f>SUM(I3:I15)</f>
-        <v>18</v>
-      </c>
       <c r="J17" s="11">
         <f>SUM(J3:J15)</f>
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="K17" s="11">
-        <f>SUM(K3:K15)</f>
-        <v>38</v>
+        <f t="shared" ref="K17:N17" si="5">SUM(K3:K15)</f>
+        <v>15</v>
       </c>
       <c r="L17" s="11">
-        <f>SUM(L3:L15)</f>
-        <v>66</v>
-      </c>
-    </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>20</v>
+      </c>
+      <c r="M17" s="11">
+        <f t="shared" si="5"/>
+        <v>23</v>
+      </c>
+      <c r="N17" s="11">
+        <f t="shared" si="5"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
       <c r="D19" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
+        <v>40</v>
+      </c>
+      <c r="C22" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>42</v>
+      </c>
+      <c r="C23" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
-        <v>36</v>
+      <c r="C24" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="E3:N15">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:N15"/>
+  <dimension ref="B2:N20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O13" sqref="O13"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1235,7 +1434,7 @@
   <sheetData>
     <row r="2" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B2" s="13" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="C2" s="14" t="s">
         <v>27</v>
@@ -1244,13 +1443,13 @@
         <v>26</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="J2" s="13" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="K2" s="14" t="s">
         <v>27</v>
@@ -1259,10 +1458,10 @@
         <v>26</v>
       </c>
       <c r="M2" s="14" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="N2" s="14" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="2:14" x14ac:dyDescent="0.25">
@@ -1283,7 +1482,7 @@
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B4" s="15" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="C4" s="11">
         <v>0</v>
@@ -1299,7 +1498,7 @@
         <v>6</v>
       </c>
       <c r="J4" s="15" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="K4" s="11">
         <v>0</v>
@@ -1329,13 +1528,11 @@
       <c r="K5" s="11"/>
       <c r="L5" s="11"/>
       <c r="M5" s="11"/>
-      <c r="N5" s="11">
-        <v>1</v>
-      </c>
+      <c r="N5" s="11"/>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B6" s="15" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="C6" s="11">
         <v>1</v>
@@ -1351,7 +1548,7 @@
         <v>6</v>
       </c>
       <c r="J6" s="15" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="K6" s="11">
         <v>1</v>
@@ -1381,13 +1578,11 @@
       <c r="K7" s="11"/>
       <c r="L7" s="11"/>
       <c r="M7" s="11"/>
-      <c r="N7" s="11">
-        <v>1</v>
-      </c>
+      <c r="N7" s="11"/>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B8" s="15" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="C8" s="11">
         <v>2</v>
@@ -1403,7 +1598,7 @@
         <v>9</v>
       </c>
       <c r="J8" s="15" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="K8" s="11">
         <v>2</v>
@@ -1433,13 +1628,11 @@
       <c r="K9" s="11"/>
       <c r="L9" s="11"/>
       <c r="M9" s="11"/>
-      <c r="N9" s="11">
-        <v>1</v>
-      </c>
+      <c r="N9" s="11"/>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B10" s="15" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="C10" s="11">
         <v>3</v>
@@ -1455,7 +1648,7 @@
         <v>9</v>
       </c>
       <c r="J10" s="15" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="K10" s="11">
         <v>3</v>
@@ -1485,13 +1678,11 @@
       <c r="K11" s="11"/>
       <c r="L11" s="11"/>
       <c r="M11" s="11"/>
-      <c r="N11" s="11">
-        <v>1</v>
-      </c>
+      <c r="N11" s="11"/>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B12" s="15" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="C12" s="11">
         <v>4</v>
@@ -1507,7 +1698,7 @@
         <v>9</v>
       </c>
       <c r="J12" s="15" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="K12" s="11">
         <v>4</v>
@@ -1533,10 +1724,10 @@
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B14" s="15" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="J14" s="15" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.25">
@@ -1552,7 +1743,71 @@
       </c>
       <c r="N15" s="14">
         <f>SUM(N4:N12)</f>
-        <v>24</v>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E17" t="s">
+        <v>50</v>
+      </c>
+      <c r="F17">
+        <f>(1/F15)</f>
+        <v>2.564102564102564E-2</v>
+      </c>
+      <c r="M17" t="s">
+        <v>50</v>
+      </c>
+      <c r="N17">
+        <f>(1/N15)</f>
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="18" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E18" t="s">
+        <v>51</v>
+      </c>
+      <c r="F18">
+        <f>F17*3</f>
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="M18" t="s">
+        <v>54</v>
+      </c>
+      <c r="N18">
+        <f>N17*1</f>
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="19" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E19" t="s">
+        <v>52</v>
+      </c>
+      <c r="F19">
+        <f>F17*6</f>
+        <v>0.15384615384615385</v>
+      </c>
+      <c r="M19" t="s">
+        <v>56</v>
+      </c>
+      <c r="N19">
+        <f>N17*3</f>
+        <v>0.15000000000000002</v>
+      </c>
+    </row>
+    <row r="20" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E20" t="s">
+        <v>57</v>
+      </c>
+      <c r="F20">
+        <f>F17*9</f>
+        <v>0.23076923076923075</v>
+      </c>
+      <c r="M20" t="s">
+        <v>55</v>
+      </c>
+      <c r="N20">
+        <f>N17*4</f>
+        <v>0.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remove token bonus from Hold completion
Not necessary now that I've worked out the cost balancing.
</commit_message>
<xml_diff>
--- a/Design Note - Cost balancing.xlsx
+++ b/Design Note - Cost balancing.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15600" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15600"/>
   </bookViews>
   <sheets>
     <sheet name="Token costs" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="59">
   <si>
     <t>Locomotion</t>
   </si>
@@ -119,9 +119,6 @@
     <t>MinTotal</t>
   </si>
   <si>
-    <t>Median</t>
-  </si>
-  <si>
     <t>Progress</t>
   </si>
   <si>
@@ -204,6 +201,12 @@
   </si>
   <si>
     <t>Shield price (9)</t>
+  </si>
+  <si>
+    <t>Kitting out a machine pistol fairly well, with all of my preferred attachments.</t>
+  </si>
+  <si>
+    <t>With the spending examples below, it's desirable for the total cost to go slightly above the total tokens of the run. This means that the player will have to make interesting decisions about what is important for their strategy and what to skip in order to afford it. For example, the player may decide not to adopt a new gun so that they can save the magazine purchase cost. Or they may hope to find guns that have compatible magazines so that they can just keep upgrading the same ones.</t>
   </si>
 </sst>
 </file>
@@ -285,7 +288,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -320,56 +323,17 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
-    <dxf>
-      <font>
-        <color theme="2"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="2"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="2"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="2"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="2"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="2"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="2"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="2"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="2"/>
-      </font>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <color theme="2"/>
@@ -677,7 +641,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -685,10 +649,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:N24"/>
+  <dimension ref="B2:N25"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -716,34 +680,34 @@
         <v>22</v>
       </c>
       <c r="E2" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="G2" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="F2" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="G2" s="11" t="s">
-        <v>38</v>
-      </c>
       <c r="H2" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I2" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J2" s="11" t="s">
         <v>28</v>
       </c>
       <c r="K2" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="L2" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="L2" s="11" t="s">
+      <c r="M2" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="M2" s="11" t="s">
-        <v>49</v>
-      </c>
       <c r="N2" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="2:14" x14ac:dyDescent="0.25">
@@ -935,7 +899,7 @@
         <v>3</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D7" s="7">
         <v>1</v>
@@ -1211,7 +1175,7 @@
         <v>12</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D13" s="10">
         <v>4</v>
@@ -1363,46 +1327,69 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="D19" t="s">
-        <v>29</v>
-      </c>
+    <row r="19" spans="2:14" ht="102" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="C19" s="17"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="17"/>
+      <c r="F19" s="17"/>
+      <c r="G19" s="17"/>
+      <c r="H19" s="17"/>
+      <c r="I19" s="17"/>
+      <c r="J19" s="16"/>
+      <c r="K19" s="16"/>
+      <c r="L19" s="16"/>
+      <c r="M19" s="16"/>
+      <c r="N19" s="16"/>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22" t="s">
         <v>40</v>
-      </c>
-      <c r="C22" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="23" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
+        <v>42</v>
+      </c>
+      <c r="C24" t="s">
         <v>43</v>
       </c>
-      <c r="C24" t="s">
-        <v>44</v>
+    </row>
+    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>52</v>
+      </c>
+      <c r="C25" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B19:I19"/>
+  </mergeCells>
   <conditionalFormatting sqref="E3:N15">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1415,7 +1402,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:N20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
@@ -1434,7 +1421,7 @@
   <sheetData>
     <row r="2" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B2" s="13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C2" s="14" t="s">
         <v>27</v>
@@ -1443,13 +1430,13 @@
         <v>26</v>
       </c>
       <c r="E2" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="F2" s="14" t="s">
-        <v>32</v>
-      </c>
       <c r="J2" s="13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K2" s="14" t="s">
         <v>27</v>
@@ -1458,10 +1445,10 @@
         <v>26</v>
       </c>
       <c r="M2" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="N2" s="14" t="s">
         <v>31</v>
-      </c>
-      <c r="N2" s="14" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="3" spans="2:14" x14ac:dyDescent="0.25">
@@ -1482,7 +1469,7 @@
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B4" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C4" s="11">
         <v>0</v>
@@ -1498,7 +1485,7 @@
         <v>6</v>
       </c>
       <c r="J4" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K4" s="11">
         <v>0</v>
@@ -1532,7 +1519,7 @@
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B6" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C6" s="11">
         <v>1</v>
@@ -1548,7 +1535,7 @@
         <v>6</v>
       </c>
       <c r="J6" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K6" s="11">
         <v>1</v>
@@ -1582,7 +1569,7 @@
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B8" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C8" s="11">
         <v>2</v>
@@ -1598,7 +1585,7 @@
         <v>9</v>
       </c>
       <c r="J8" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K8" s="11">
         <v>2</v>
@@ -1632,7 +1619,7 @@
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B10" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C10" s="11">
         <v>3</v>
@@ -1648,7 +1635,7 @@
         <v>9</v>
       </c>
       <c r="J10" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K10" s="11">
         <v>3</v>
@@ -1682,7 +1669,7 @@
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B12" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C12" s="11">
         <v>4</v>
@@ -1698,7 +1685,7 @@
         <v>9</v>
       </c>
       <c r="J12" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K12" s="11">
         <v>4</v>
@@ -1724,10 +1711,10 @@
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B14" s="15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J14" s="15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.25">
@@ -1748,14 +1735,14 @@
     </row>
     <row r="17" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F17">
         <f>(1/F15)</f>
         <v>2.564102564102564E-2</v>
       </c>
       <c r="M17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="N17">
         <f>(1/N15)</f>
@@ -1764,14 +1751,14 @@
     </row>
     <row r="18" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F18">
         <f>F17*3</f>
         <v>7.6923076923076927E-2</v>
       </c>
       <c r="M18" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="N18">
         <f>N17*1</f>
@@ -1780,14 +1767,14 @@
     </row>
     <row r="19" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E19" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F19">
         <f>F17*6</f>
         <v>0.15384615384615385</v>
       </c>
       <c r="M19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="N19">
         <f>N17*3</f>
@@ -1796,14 +1783,14 @@
     </row>
     <row r="20" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F20">
         <f>F17*9</f>
         <v>0.23076923076923075</v>
       </c>
       <c r="M20" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="N20">
         <f>N17*4</f>

</xml_diff>

<commit_message>
Split shop pools evenly and allow all to spawn throughout game
</commit_message>
<xml_diff>
--- a/Design Note - Cost balancing.xlsx
+++ b/Design Note - Cost balancing.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="60">
   <si>
     <t>Locomotion</t>
   </si>
@@ -207,6 +207,9 @@
   </si>
   <si>
     <t>Claymore</t>
+  </si>
+  <si>
+    <t>Equipment</t>
   </si>
 </sst>
 </file>
@@ -238,7 +241,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -266,6 +269,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -302,7 +311,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -327,9 +336,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -359,29 +365,26 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <font>
-        <color theme="2"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="2"/>
-      </font>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <color theme="2"/>
@@ -689,7 +692,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -700,7 +703,7 @@
   <dimension ref="B2:N26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -804,29 +807,29 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:14" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:14" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="20" t="s">
+      <c r="C4" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="21">
-        <v>1</v>
-      </c>
-      <c r="E4" s="14">
-        <v>0</v>
-      </c>
-      <c r="F4" s="14">
-        <v>0</v>
-      </c>
-      <c r="G4" s="14">
-        <v>0</v>
-      </c>
-      <c r="H4" s="14">
-        <v>0</v>
-      </c>
-      <c r="I4" s="14">
+      <c r="D4" s="20">
+        <v>1</v>
+      </c>
+      <c r="E4" s="13">
+        <v>0</v>
+      </c>
+      <c r="F4" s="13">
+        <v>0</v>
+      </c>
+      <c r="G4" s="13">
+        <v>0</v>
+      </c>
+      <c r="H4" s="13">
+        <v>0</v>
+      </c>
+      <c r="I4" s="13">
         <v>0</v>
       </c>
       <c r="J4" s="6">
@@ -850,30 +853,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:14" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="D5" s="27">
-        <v>4</v>
-      </c>
-      <c r="E5" s="28">
-        <v>0</v>
-      </c>
-      <c r="F5" s="28">
-        <v>0</v>
-      </c>
-      <c r="G5" s="28">
-        <v>0</v>
-      </c>
-      <c r="H5" s="28">
-        <v>0</v>
-      </c>
-      <c r="I5" s="28">
-        <v>0</v>
+    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B5" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="22">
+        <v>1</v>
+      </c>
+      <c r="E5" s="5">
+        <v>0</v>
+      </c>
+      <c r="F5" s="5">
+        <v>0</v>
+      </c>
+      <c r="G5" s="5">
+        <v>1</v>
+      </c>
+      <c r="H5" s="5">
+        <v>1</v>
+      </c>
+      <c r="I5" s="5">
+        <v>1</v>
       </c>
       <c r="J5" s="6">
         <f t="shared" si="1"/>
@@ -889,21 +892,21 @@
       </c>
       <c r="M5" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N5" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="23">
+      <c r="C6" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="22">
         <v>1</v>
       </c>
       <c r="E6" s="5">
@@ -913,10 +916,10 @@
         <v>0</v>
       </c>
       <c r="G6" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H6" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I6" s="5">
         <v>1</v>
@@ -935,36 +938,36 @@
       </c>
       <c r="M6" s="6">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N6" s="6">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B7" s="22" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="D7" s="23">
-        <v>1</v>
-      </c>
-      <c r="E7" s="5">
-        <v>0</v>
-      </c>
-      <c r="F7" s="5">
-        <v>0</v>
-      </c>
-      <c r="G7" s="5">
-        <v>0</v>
-      </c>
-      <c r="H7" s="5">
-        <v>0</v>
-      </c>
-      <c r="I7" s="5">
+      <c r="C7" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="24">
+        <v>1</v>
+      </c>
+      <c r="E7" s="13">
+        <v>0</v>
+      </c>
+      <c r="F7" s="13">
+        <v>0</v>
+      </c>
+      <c r="G7" s="13">
+        <v>1</v>
+      </c>
+      <c r="H7" s="13">
+        <v>1</v>
+      </c>
+      <c r="I7" s="13">
         <v>1</v>
       </c>
       <c r="J7" s="6">
@@ -981,21 +984,21 @@
       </c>
       <c r="M7" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N7" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B8" s="22" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" s="22" t="s">
-        <v>1</v>
-      </c>
-      <c r="D8" s="23">
+      <c r="B8" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="C8" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" s="31">
         <v>1</v>
       </c>
       <c r="E8" s="5">
@@ -1014,81 +1017,81 @@
         <v>0</v>
       </c>
       <c r="J8" s="6">
-        <f t="shared" si="1"/>
+        <f>D8*E8</f>
         <v>0</v>
       </c>
       <c r="K8" s="6">
-        <f t="shared" si="0"/>
+        <f>E8*F8</f>
         <v>0</v>
       </c>
       <c r="L8" s="6">
-        <f t="shared" si="0"/>
+        <f>F8*G8</f>
         <v>0</v>
       </c>
       <c r="M8" s="6">
-        <f t="shared" si="0"/>
+        <f>G8*H8</f>
         <v>0</v>
       </c>
       <c r="N8" s="6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="2:14" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="22" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" s="24" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="25">
-        <v>1</v>
-      </c>
-      <c r="E9" s="14">
-        <v>0</v>
-      </c>
-      <c r="F9" s="14">
-        <v>0</v>
-      </c>
-      <c r="G9" s="14">
-        <v>1</v>
-      </c>
-      <c r="H9" s="14">
-        <v>1</v>
-      </c>
-      <c r="I9" s="14">
-        <v>1</v>
+        <f>H8*I8</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14" s="26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="C9" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="D9" s="30">
+        <v>4</v>
+      </c>
+      <c r="E9" s="25">
+        <v>0</v>
+      </c>
+      <c r="F9" s="25">
+        <v>0</v>
+      </c>
+      <c r="G9" s="25">
+        <v>0</v>
+      </c>
+      <c r="H9" s="25">
+        <v>0</v>
+      </c>
+      <c r="I9" s="25">
+        <v>0</v>
       </c>
       <c r="J9" s="6">
-        <f t="shared" si="1"/>
+        <f>D9*E9</f>
         <v>0</v>
       </c>
       <c r="K9" s="6">
-        <f t="shared" si="0"/>
+        <f>E9*F9</f>
         <v>0</v>
       </c>
       <c r="L9" s="6">
-        <f t="shared" si="0"/>
+        <f>F9*G9</f>
         <v>0</v>
       </c>
       <c r="M9" s="6">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f>G9*H9</f>
+        <v>0</v>
       </c>
       <c r="N9" s="6">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f>H9*I9</f>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B10" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" s="4">
-        <v>1</v>
+      <c r="B10" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="C10" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="31">
+        <v>4</v>
       </c>
       <c r="E10" s="5">
         <v>0</v>
@@ -1106,23 +1109,23 @@
         <v>0</v>
       </c>
       <c r="J10" s="6">
-        <f t="shared" si="1"/>
+        <f>D10*E10</f>
         <v>0</v>
       </c>
       <c r="K10" s="6">
-        <f t="shared" si="0"/>
+        <f>E10*F10</f>
         <v>0</v>
       </c>
       <c r="L10" s="6">
-        <f t="shared" si="0"/>
+        <f>F10*G10</f>
         <v>0</v>
       </c>
       <c r="M10" s="6">
-        <f t="shared" si="0"/>
+        <f>G10*H10</f>
         <v>0</v>
       </c>
       <c r="N10" s="6">
-        <f t="shared" si="0"/>
+        <f>H10*I10</f>
         <v>0</v>
       </c>
     </row>
@@ -1131,16 +1134,16 @@
         <v>8</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D11" s="4">
         <v>1</v>
       </c>
       <c r="E11" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F11" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G11" s="5">
         <v>0</v>
@@ -1149,15 +1152,15 @@
         <v>0</v>
       </c>
       <c r="I11" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J11" s="6">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K11" s="6">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L11" s="6">
         <f t="shared" si="0"/>
@@ -1172,121 +1175,121 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:14" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="D12" s="13">
-        <v>1</v>
-      </c>
-      <c r="E12" s="14">
-        <v>0</v>
-      </c>
-      <c r="F12" s="14">
-        <v>0</v>
-      </c>
-      <c r="G12" s="14">
-        <v>0</v>
-      </c>
-      <c r="H12" s="14">
-        <v>0</v>
-      </c>
-      <c r="I12" s="14">
-        <v>0</v>
+      <c r="C12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="4">
+        <v>1</v>
+      </c>
+      <c r="E12" s="5">
+        <v>1</v>
+      </c>
+      <c r="F12" s="5">
+        <v>1</v>
+      </c>
+      <c r="G12" s="5">
+        <v>0</v>
+      </c>
+      <c r="H12" s="5">
+        <v>0</v>
+      </c>
+      <c r="I12" s="5">
+        <v>1</v>
       </c>
       <c r="J12" s="6">
-        <f>D12*E12</f>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="K12" s="6">
-        <f>E12*F12</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="L12" s="6">
-        <f>F12*G12</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="M12" s="6">
-        <f>G12*H12</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N12" s="6">
-        <f>H12*I12</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:14" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D13" s="4">
+      <c r="C13" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" s="12">
+        <v>1</v>
+      </c>
+      <c r="E13" s="13">
+        <v>0</v>
+      </c>
+      <c r="F13" s="13">
+        <v>0</v>
+      </c>
+      <c r="G13" s="13">
+        <v>0</v>
+      </c>
+      <c r="H13" s="13">
+        <v>0</v>
+      </c>
+      <c r="I13" s="13">
+        <v>0</v>
+      </c>
+      <c r="J13" s="6">
+        <f>D13*E13</f>
+        <v>0</v>
+      </c>
+      <c r="K13" s="6">
+        <f>E13*F13</f>
+        <v>0</v>
+      </c>
+      <c r="L13" s="6">
+        <f>F13*G13</f>
+        <v>0</v>
+      </c>
+      <c r="M13" s="6">
+        <f>G13*H13</f>
+        <v>0</v>
+      </c>
+      <c r="N13" s="6">
+        <f>H13*I13</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:14" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="16">
         <v>4</v>
       </c>
-      <c r="E13" s="5">
-        <v>0</v>
-      </c>
-      <c r="F13" s="5">
-        <v>0</v>
-      </c>
-      <c r="G13" s="5">
-        <v>0</v>
-      </c>
-      <c r="H13" s="5">
-        <v>0</v>
-      </c>
-      <c r="I13" s="5">
-        <v>0</v>
-      </c>
-      <c r="J13" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K13" s="6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L13" s="6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M13" s="6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="N13" s="6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="2:14" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="D14" s="17">
-        <v>4</v>
-      </c>
-      <c r="E14" s="18">
-        <v>0</v>
-      </c>
-      <c r="F14" s="18">
-        <v>1</v>
-      </c>
-      <c r="G14" s="18">
-        <v>0</v>
-      </c>
-      <c r="H14" s="18">
-        <v>1</v>
-      </c>
-      <c r="I14" s="18">
+      <c r="E14" s="17">
+        <v>0</v>
+      </c>
+      <c r="F14" s="17">
+        <v>1</v>
+      </c>
+      <c r="G14" s="17">
+        <v>0</v>
+      </c>
+      <c r="H14" s="17">
+        <v>1</v>
+      </c>
+      <c r="I14" s="17">
         <v>0</v>
       </c>
       <c r="J14" s="6">
@@ -1401,37 +1404,37 @@
         <v>24</v>
       </c>
       <c r="J18" s="5">
-        <f>SUM(J8:J16)</f>
+        <f>SUM(J7:J16)</f>
         <v>11</v>
       </c>
       <c r="K18" s="5">
-        <f>SUM(K8:K16)</f>
+        <f>SUM(K7:K16)</f>
         <v>26</v>
       </c>
       <c r="L18" s="5">
-        <f>SUM(L8:L16)</f>
+        <f>SUM(L7:L16)</f>
         <v>20</v>
       </c>
       <c r="M18" s="5">
-        <f>SUM(M8:M16)</f>
+        <f>SUM(M7:M16)</f>
         <v>26</v>
       </c>
       <c r="N18" s="5">
-        <f>SUM(N8:N16)</f>
+        <f>SUM(N7:N16)</f>
         <v>26</v>
       </c>
     </row>
     <row r="20" spans="2:14" ht="102" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="11" t="s">
+      <c r="B20" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="11"/>
-      <c r="I20" s="11"/>
+      <c r="C20" s="27"/>
+      <c r="D20" s="27"/>
+      <c r="E20" s="27"/>
+      <c r="F20" s="27"/>
+      <c r="G20" s="27"/>
+      <c r="H20" s="27"/>
+      <c r="I20" s="27"/>
       <c r="J20" s="10"/>
       <c r="K20" s="10"/>
       <c r="L20" s="10"/>

</xml_diff>

<commit_message>
Increase cost of 1-token items to 2 tokens
I got some of the formulas in my spreadsheet wrong and made them too cheap.
</commit_message>
<xml_diff>
--- a/Design Note - Cost balancing.xlsx
+++ b/Design Note - Cost balancing.xlsx
@@ -188,9 +188,6 @@
     <t>Ideal</t>
   </si>
   <si>
-    <t>Base price (1)</t>
-  </si>
-  <si>
     <t>Shield price (4)</t>
   </si>
   <si>
@@ -210,6 +207,9 @@
   </si>
   <si>
     <t>Equipment</t>
+  </si>
+  <si>
+    <t>Base price (2)</t>
   </si>
 </sst>
 </file>
@@ -320,9 +320,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -342,6 +339,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -666,7 +666,7 @@
   <dimension ref="B2:N26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -725,14 +725,14 @@
       </c>
     </row>
     <row r="3" spans="2:14" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="11" t="s">
+      <c r="B3" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="12">
-        <v>1</v>
+      <c r="D3" s="11">
+        <v>2</v>
       </c>
       <c r="E3" s="6">
         <v>1</v>
@@ -749,220 +749,220 @@
       <c r="I3" s="6">
         <v>1</v>
       </c>
-      <c r="J3" s="13">
+      <c r="J3" s="12">
         <f>D3*E3</f>
-        <v>1</v>
-      </c>
-      <c r="K3" s="13">
-        <f t="shared" ref="K3:N16" si="0">E3*F3</f>
-        <v>1</v>
-      </c>
-      <c r="L3" s="13">
+        <v>2</v>
+      </c>
+      <c r="K3" s="12">
+        <f>D3*F3</f>
+        <v>2</v>
+      </c>
+      <c r="L3" s="12">
+        <f>D3*G3</f>
+        <v>2</v>
+      </c>
+      <c r="M3" s="12">
+        <f>D3*H3</f>
+        <v>2</v>
+      </c>
+      <c r="N3" s="12">
+        <f>D3*I3</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:14" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="11">
+        <v>2</v>
+      </c>
+      <c r="E4" s="6">
+        <v>0</v>
+      </c>
+      <c r="F4" s="6">
+        <v>0</v>
+      </c>
+      <c r="G4" s="6">
+        <v>0</v>
+      </c>
+      <c r="H4" s="6">
+        <v>0</v>
+      </c>
+      <c r="I4" s="6">
+        <v>0</v>
+      </c>
+      <c r="J4" s="12">
+        <f>D4*E4</f>
+        <v>0</v>
+      </c>
+      <c r="K4" s="12">
+        <f t="shared" ref="K4:K16" si="0">D4*F4</f>
+        <v>0</v>
+      </c>
+      <c r="L4" s="12">
+        <f t="shared" ref="L4:L16" si="1">D4*G4</f>
+        <v>0</v>
+      </c>
+      <c r="M4" s="12">
+        <f t="shared" ref="M4:M16" si="2">D4*H4</f>
+        <v>0</v>
+      </c>
+      <c r="N4" s="12">
+        <f t="shared" ref="N4:N16" si="3">D4*I4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="2:14" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" s="11">
+        <v>2</v>
+      </c>
+      <c r="E5" s="6">
+        <v>0</v>
+      </c>
+      <c r="F5" s="6">
+        <v>0</v>
+      </c>
+      <c r="G5" s="6">
+        <v>0</v>
+      </c>
+      <c r="H5" s="6">
+        <v>0</v>
+      </c>
+      <c r="I5" s="6">
+        <v>0</v>
+      </c>
+      <c r="J5" s="12">
+        <f>D5*E5</f>
+        <v>0</v>
+      </c>
+      <c r="K5" s="12">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="M3" s="13">
+        <v>0</v>
+      </c>
+      <c r="L5" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M5" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N5" s="12">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:14" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="14">
+        <v>2</v>
+      </c>
+      <c r="E6" s="6">
+        <v>0</v>
+      </c>
+      <c r="F6" s="6">
+        <v>0</v>
+      </c>
+      <c r="G6" s="6">
+        <v>1</v>
+      </c>
+      <c r="H6" s="6">
+        <v>1</v>
+      </c>
+      <c r="I6" s="6">
+        <v>1</v>
+      </c>
+      <c r="J6" s="12">
+        <f>D6*E6</f>
+        <v>0</v>
+      </c>
+      <c r="K6" s="12">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="N3" s="13">
+        <v>0</v>
+      </c>
+      <c r="L6" s="12">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="M6" s="12">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="N6" s="12">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="14">
+        <v>2</v>
+      </c>
+      <c r="E7" s="6">
+        <v>1</v>
+      </c>
+      <c r="F7" s="6">
+        <v>1</v>
+      </c>
+      <c r="G7" s="6">
+        <v>0</v>
+      </c>
+      <c r="H7" s="6">
+        <v>0</v>
+      </c>
+      <c r="I7" s="6">
+        <v>1</v>
+      </c>
+      <c r="J7" s="12">
+        <f>D7*E7</f>
+        <v>2</v>
+      </c>
+      <c r="K7" s="12">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="2:14" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="12">
-        <v>1</v>
-      </c>
-      <c r="E4" s="6">
-        <v>0</v>
-      </c>
-      <c r="F4" s="6">
-        <v>0</v>
-      </c>
-      <c r="G4" s="6">
-        <v>0</v>
-      </c>
-      <c r="H4" s="6">
-        <v>0</v>
-      </c>
-      <c r="I4" s="6">
-        <v>0</v>
-      </c>
-      <c r="J4" s="13">
-        <f>D4*E4</f>
-        <v>0</v>
-      </c>
-      <c r="K4" s="13">
-        <f>E4*F4</f>
-        <v>0</v>
-      </c>
-      <c r="L4" s="13">
-        <f>F4*G4</f>
-        <v>0</v>
-      </c>
-      <c r="M4" s="13">
-        <f>G4*H4</f>
-        <v>0</v>
-      </c>
-      <c r="N4" s="13">
-        <f>H4*I4</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="2:14" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="D5" s="12">
-        <v>1</v>
-      </c>
-      <c r="E5" s="6">
-        <v>0</v>
-      </c>
-      <c r="F5" s="6">
-        <v>0</v>
-      </c>
-      <c r="G5" s="6">
-        <v>0</v>
-      </c>
-      <c r="H5" s="6">
-        <v>0</v>
-      </c>
-      <c r="I5" s="6">
-        <v>0</v>
-      </c>
-      <c r="J5" s="13">
-        <f>D5*E5</f>
-        <v>0</v>
-      </c>
-      <c r="K5" s="13">
-        <f>E5*F5</f>
-        <v>0</v>
-      </c>
-      <c r="L5" s="13">
-        <f>F5*G5</f>
-        <v>0</v>
-      </c>
-      <c r="M5" s="13">
-        <f>G5*H5</f>
-        <v>0</v>
-      </c>
-      <c r="N5" s="13">
-        <f>H5*I5</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="2:14" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="L7" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M7" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N7" s="12">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="15">
-        <v>1</v>
-      </c>
-      <c r="E6" s="6">
-        <v>0</v>
-      </c>
-      <c r="F6" s="6">
-        <v>0</v>
-      </c>
-      <c r="G6" s="6">
-        <v>1</v>
-      </c>
-      <c r="H6" s="6">
-        <v>1</v>
-      </c>
-      <c r="I6" s="6">
-        <v>1</v>
-      </c>
-      <c r="J6" s="13">
-        <f>D6*E6</f>
-        <v>0</v>
-      </c>
-      <c r="K6" s="13">
-        <f>E6*F6</f>
-        <v>0</v>
-      </c>
-      <c r="L6" s="13">
-        <f>F6*G6</f>
-        <v>0</v>
-      </c>
-      <c r="M6" s="13">
-        <f>G6*H6</f>
-        <v>1</v>
-      </c>
-      <c r="N6" s="13">
-        <f>H6*I6</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="2:14" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="15">
-        <v>1</v>
-      </c>
-      <c r="E7" s="6">
-        <v>1</v>
-      </c>
-      <c r="F7" s="6">
-        <v>1</v>
-      </c>
-      <c r="G7" s="6">
-        <v>0</v>
-      </c>
-      <c r="H7" s="6">
-        <v>0</v>
-      </c>
-      <c r="I7" s="6">
-        <v>1</v>
-      </c>
-      <c r="J7" s="13">
-        <f>D7*E7</f>
-        <v>1</v>
-      </c>
-      <c r="K7" s="13">
-        <f>E7*F7</f>
-        <v>1</v>
-      </c>
-      <c r="L7" s="13">
-        <f>F7*G7</f>
-        <v>0</v>
-      </c>
-      <c r="M7" s="13">
-        <f>G7*H7</f>
-        <v>0</v>
-      </c>
-      <c r="N7" s="13">
-        <f>H7*I7</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="2:14" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" s="14" t="s">
+      <c r="C8" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="15">
-        <v>1</v>
+      <c r="D8" s="14">
+        <v>2</v>
       </c>
       <c r="E8" s="6">
         <v>0</v>
@@ -979,36 +979,36 @@
       <c r="I8" s="6">
         <v>0</v>
       </c>
-      <c r="J8" s="13">
-        <f t="shared" ref="J8:J16" si="1">D8*E8</f>
-        <v>0</v>
-      </c>
-      <c r="K8" s="13">
+      <c r="J8" s="12">
+        <f t="shared" ref="J8:J16" si="4">D8*E8</f>
+        <v>0</v>
+      </c>
+      <c r="K8" s="12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L8" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M8" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="N8" s="13">
-        <f t="shared" si="0"/>
+      <c r="L8" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M8" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N8" s="12">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="2:14" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B9" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>1</v>
       </c>
       <c r="D9" s="9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E9" s="6">
         <v>0</v>
@@ -1025,36 +1025,36 @@
       <c r="I9" s="6">
         <v>0</v>
       </c>
-      <c r="J9" s="13">
-        <f>D9*E9</f>
-        <v>0</v>
-      </c>
-      <c r="K9" s="13">
-        <f>E9*F9</f>
-        <v>0</v>
-      </c>
-      <c r="L9" s="13">
-        <f>F9*G9</f>
-        <v>0</v>
-      </c>
-      <c r="M9" s="13">
-        <f>G9*H9</f>
-        <v>0</v>
-      </c>
-      <c r="N9" s="13">
-        <f>H9*I9</f>
+      <c r="J9" s="12">
+        <f t="shared" ref="J9:J11" si="5">D9*E9</f>
+        <v>0</v>
+      </c>
+      <c r="K9" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L9" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M9" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N9" s="12">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="2:14" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B10" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>2</v>
       </c>
       <c r="D10" s="9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E10" s="6">
         <v>0</v>
@@ -1071,35 +1071,35 @@
       <c r="I10" s="6">
         <v>1</v>
       </c>
-      <c r="J10" s="13">
-        <f>D10*E10</f>
-        <v>0</v>
-      </c>
-      <c r="K10" s="13">
-        <f>E10*F10</f>
-        <v>0</v>
-      </c>
-      <c r="L10" s="13">
-        <f>F10*G10</f>
-        <v>0</v>
-      </c>
-      <c r="M10" s="13">
-        <f>G10*H10</f>
-        <v>0</v>
-      </c>
-      <c r="N10" s="13">
-        <f>H10*I10</f>
-        <v>0</v>
+      <c r="J10" s="12">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K10" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L10" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M10" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N10" s="12">
+        <f t="shared" si="3"/>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="2:14" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="19" t="s">
+      <c r="B11" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="19" t="s">
-        <v>58</v>
-      </c>
-      <c r="D11" s="20">
+      <c r="C11" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="D11" s="19">
         <v>4</v>
       </c>
       <c r="E11" s="6">
@@ -1117,35 +1117,35 @@
       <c r="I11" s="6">
         <v>0</v>
       </c>
-      <c r="J11" s="13">
-        <f>D11*E11</f>
-        <v>0</v>
-      </c>
-      <c r="K11" s="13">
-        <f>E11*F11</f>
-        <v>0</v>
-      </c>
-      <c r="L11" s="13">
-        <f>F11*G11</f>
-        <v>0</v>
-      </c>
-      <c r="M11" s="13">
-        <f>G11*H11</f>
-        <v>0</v>
-      </c>
-      <c r="N11" s="13">
-        <f>H11*I11</f>
+      <c r="J11" s="12">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K11" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L11" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M11" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N11" s="12">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="2:14" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="19" t="s">
+      <c r="B12" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="19" t="s">
+      <c r="C12" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="D12" s="20">
+      <c r="D12" s="19">
         <v>4</v>
       </c>
       <c r="E12" s="6">
@@ -1163,116 +1163,116 @@
       <c r="I12" s="6">
         <v>0</v>
       </c>
-      <c r="J12" s="13">
-        <f t="shared" ref="J12:N12" si="2">D12*E12</f>
-        <v>0</v>
-      </c>
-      <c r="K12" s="13">
+      <c r="J12" s="12">
+        <f t="shared" ref="J12" si="6">D12*E12</f>
+        <v>0</v>
+      </c>
+      <c r="K12" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L12" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M12" s="12">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="L12" s="13">
+      <c r="N12" s="12">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:14" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="19">
+        <v>2</v>
+      </c>
+      <c r="E13" s="6">
+        <v>0</v>
+      </c>
+      <c r="F13" s="6">
+        <v>0</v>
+      </c>
+      <c r="G13" s="6">
+        <v>1</v>
+      </c>
+      <c r="H13" s="6">
+        <v>1</v>
+      </c>
+      <c r="I13" s="6">
+        <v>1</v>
+      </c>
+      <c r="J13" s="12">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="K13" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L13" s="12">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="M13" s="12">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M12" s="13">
+        <v>2</v>
+      </c>
+      <c r="N13" s="12">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="2:14" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="17">
+        <v>4</v>
+      </c>
+      <c r="E14" s="6">
+        <v>0</v>
+      </c>
+      <c r="F14" s="6">
+        <v>1</v>
+      </c>
+      <c r="G14" s="6">
+        <v>0</v>
+      </c>
+      <c r="H14" s="6">
+        <v>1</v>
+      </c>
+      <c r="I14" s="6">
+        <v>0</v>
+      </c>
+      <c r="J14" s="12">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="K14" s="12">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="L14" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M14" s="12">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N12" s="13">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="2:14" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13" s="20">
-        <v>1</v>
-      </c>
-      <c r="E13" s="6">
-        <v>0</v>
-      </c>
-      <c r="F13" s="6">
-        <v>0</v>
-      </c>
-      <c r="G13" s="6">
-        <v>1</v>
-      </c>
-      <c r="H13" s="6">
-        <v>1</v>
-      </c>
-      <c r="I13" s="6">
-        <v>1</v>
-      </c>
-      <c r="J13" s="13">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K13" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L13" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M13" s="13">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="N13" s="13">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="2:14" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="D14" s="18">
         <v>4</v>
       </c>
-      <c r="E14" s="6">
-        <v>0</v>
-      </c>
-      <c r="F14" s="6">
-        <v>1</v>
-      </c>
-      <c r="G14" s="6">
-        <v>0</v>
-      </c>
-      <c r="H14" s="6">
-        <v>1</v>
-      </c>
-      <c r="I14" s="6">
-        <v>0</v>
-      </c>
-      <c r="J14" s="13">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K14" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L14" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M14" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="N14" s="13">
-        <f t="shared" si="0"/>
+      <c r="N14" s="12">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -1298,25 +1298,25 @@
       <c r="I15" s="6">
         <v>4</v>
       </c>
-      <c r="J15" s="13">
+      <c r="J15" s="12">
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
+      <c r="K15" s="12">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="L15" s="12">
         <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-      <c r="K15" s="13">
-        <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-      <c r="L15" s="13">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="M15" s="13">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="N15" s="13">
-        <f t="shared" si="0"/>
-        <v>16</v>
+        <v>8</v>
+      </c>
+      <c r="M15" s="12">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="N15" s="12">
+        <f t="shared" si="3"/>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="2:14" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -1341,24 +1341,24 @@
       <c r="I16" s="6">
         <v>3</v>
       </c>
-      <c r="J16" s="13">
+      <c r="J16" s="12">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="K16" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L16" s="12">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K16" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L16" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M16" s="13">
-        <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="N16" s="13">
-        <f t="shared" si="0"/>
+      <c r="M16" s="12">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="N16" s="12">
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
     </row>
@@ -1371,36 +1371,36 @@
       </c>
       <c r="J18" s="1">
         <f>SUM(J6:J16)</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="K18" s="1">
         <f>SUM(K6:K16)</f>
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="L18" s="1">
         <f>SUM(L6:L16)</f>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M18" s="1">
         <f>SUM(M6:M16)</f>
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="N18" s="1">
         <f>SUM(N6:N16)</f>
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="20" spans="2:14" ht="102" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="10"/>
-      <c r="G20" s="10"/>
-      <c r="H20" s="10"/>
-      <c r="I20" s="10"/>
+      <c r="B20" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="C20" s="20"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="20"/>
+      <c r="H20" s="20"/>
+      <c r="I20" s="20"/>
       <c r="J20" s="5"/>
       <c r="K20" s="5"/>
       <c r="L20" s="5"/>
@@ -1444,7 +1444,7 @@
         <v>51</v>
       </c>
       <c r="C26" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1466,7 +1466,7 @@
   <dimension ref="B2:N20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P21" sqref="P21"/>
+      <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1821,11 +1821,11 @@
         <v>7.6923076923076927E-2</v>
       </c>
       <c r="M18" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="N18">
-        <f>N17*1</f>
-        <v>0.05</v>
+        <f>N17*2</f>
+        <v>0.1</v>
       </c>
     </row>
     <row r="19" spans="5:14" x14ac:dyDescent="0.25">
@@ -1837,7 +1837,7 @@
         <v>0.15384615384615385</v>
       </c>
       <c r="M19" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="N19">
         <f>N17*4</f>
@@ -1846,14 +1846,14 @@
     </row>
     <row r="20" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E20" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F20">
         <f>F17*9</f>
         <v>0.23076923076923075</v>
       </c>
       <c r="M20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="N20">
         <f>N17*4</f>

</xml_diff>